<commit_message>
Ajustes para a nova versão do publisher
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-BRAlergiaReacaoAdversa-1.0.xlsx
+++ b/docs/StructureDefinition-BRAlergiaReacaoAdversa-1.0.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -2090,15 +2090,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="75.68359375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="54.69921875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="17.4921875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="37.5859375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.9296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.47265625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.87890625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.2734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.7265625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="72.171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="52.16015625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="35.84375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.65234375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.265625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65234375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.1796875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2109,25 +2109,25 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="36.22265625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.4609375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="15.86328125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.203125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="116.19140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="79.3515625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.52734375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="38.34375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="15.06640625" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.421875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="37.9765625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.28515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.6875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="34.54296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.7421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.12890625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.40625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="15.85546875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="110.80078125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="75.66796875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.2734375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.1171875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="36.56640625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.3671875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.84375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="36.2109375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.85546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.23828125" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="32.4453125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="42.12109375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="30.9375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="40.16796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6824,7 +6824,7 @@
         <v>76</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>78</v>

</xml_diff>